<commit_message>
revisión de algoritmos de estimacion de SPO2 y tablas resumen de resultados
</commit_message>
<xml_diff>
--- a/Código/procesamiento/SpO2/SpO2_estimaciones_filtradas.xlsx
+++ b/Código/procesamiento/SpO2/SpO2_estimaciones_filtradas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="21">
   <si>
     <t>Archivo</t>
   </si>
@@ -58,9 +58,6 @@
     <t>raw_data_96_69.csv</t>
   </si>
   <si>
-    <t>raw_data_96_81.csv</t>
-  </si>
-  <si>
     <t>raw_data_97_119.csv</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
   </si>
   <si>
     <t>raw_data_98_91.csv</t>
-  </si>
-  <si>
-    <t>raw_data_99_73.csv</t>
   </si>
   <si>
     <t>raw_data_99_75.csv</t>
@@ -440,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E108"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -468,16 +462,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>5147</v>
+        <v>14142</v>
       </c>
       <c r="C2">
         <v>91</v>
       </c>
       <c r="D2">
-        <v>95.13339758921427</v>
+        <v>95.23590061801499</v>
       </c>
       <c r="E2">
-        <v>1.80588056770811</v>
+        <v>1.698671040670436</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -485,16 +479,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>9411</v>
+        <v>18405</v>
       </c>
       <c r="C3">
         <v>91</v>
       </c>
       <c r="D3">
-        <v>95.16098800363397</v>
+        <v>95.2574493818986</v>
       </c>
       <c r="E3">
-        <v>1.777023320119256</v>
+        <v>1.676132850226336</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -502,16 +496,16 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>13675</v>
+        <v>22669</v>
       </c>
       <c r="C4">
         <v>91</v>
       </c>
       <c r="D4">
-        <v>95.23358491049031</v>
+        <v>95.27055795107806</v>
       </c>
       <c r="E4">
-        <v>1.701093075525257</v>
+        <v>1.662422391927552</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -519,50 +513,50 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>17939</v>
+        <v>26933</v>
       </c>
       <c r="C5">
         <v>91</v>
       </c>
       <c r="D5">
-        <v>95.25519276588284</v>
+        <v>95.28852245306796</v>
       </c>
       <c r="E5">
-        <v>1.678493080344273</v>
+        <v>1.643633037268108</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>22203</v>
+        <v>5147</v>
       </c>
       <c r="C6">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D6">
-        <v>95.26983534187066</v>
+        <v>96.71170788887837</v>
       </c>
       <c r="E6">
-        <v>1.663178180241968</v>
+        <v>0.1551010470888334</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>26466</v>
+        <v>9411</v>
       </c>
       <c r="C7">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D7">
-        <v>95.28590146856375</v>
+        <v>96.74046166974574</v>
       </c>
       <c r="E7">
-        <v>1.646374366108404</v>
+        <v>0.1250270162684484</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -570,1716 +564,1138 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>5147</v>
+        <v>13675</v>
       </c>
       <c r="C8">
         <v>92</v>
       </c>
       <c r="D8">
-        <v>96.71170788887837</v>
+        <v>96.75339889704543</v>
       </c>
       <c r="E8">
-        <v>0.1551010470888334</v>
+        <v>0.111495767131644</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>9411</v>
+        <v>14141</v>
       </c>
       <c r="C9">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D9">
-        <v>96.74046166974574</v>
+        <v>96.78671768049405</v>
       </c>
       <c r="E9">
-        <v>0.1250270162684484</v>
+        <v>0.07664712844467356</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>13675</v>
+        <v>18405</v>
       </c>
       <c r="C10">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D10">
-        <v>96.75339889704543</v>
+        <v>96.72692418245101</v>
       </c>
       <c r="E10">
-        <v>0.111495767131644</v>
+        <v>0.1391860867576419</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>17939</v>
+        <v>22669</v>
       </c>
       <c r="C11">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D11">
-        <v>96.72559204698759</v>
+        <v>96.65906392292439</v>
       </c>
       <c r="E11">
-        <v>0.1405793881522993</v>
+        <v>0.2101621975479604</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>22203</v>
+        <v>5147</v>
       </c>
       <c r="C12">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D12">
-        <v>96.75313232336028</v>
+        <v>95.8966790792869</v>
       </c>
       <c r="E12">
-        <v>0.1117745807339485</v>
+        <v>1.007552474336466</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B13">
-        <v>26466</v>
+        <v>9411</v>
       </c>
       <c r="C13">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D13">
-        <v>96.7480483073756</v>
+        <v>95.90568450751066</v>
       </c>
       <c r="E13">
-        <v>0.1170920328672737</v>
+        <v>0.9981335555792762</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14">
-        <v>5147</v>
+        <v>13675</v>
       </c>
       <c r="C14">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D14">
-        <v>95.8102976696071</v>
+        <v>95.91581714251014</v>
       </c>
       <c r="E14">
-        <v>1.097900146839142</v>
+        <v>0.9875356735591134</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15">
-        <v>9411</v>
+        <v>17939</v>
       </c>
       <c r="C15">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D15">
-        <v>95.59256316529444</v>
+        <v>95.92117144678738</v>
       </c>
       <c r="E15">
-        <v>1.325632083156124</v>
+        <v>0.9819355226572629</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B16">
-        <v>13675</v>
+        <v>22203</v>
       </c>
       <c r="C16">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D16">
-        <v>96.66405137600034</v>
+        <v>95.9284816007417</v>
       </c>
       <c r="E16">
-        <v>0.2049457420768244</v>
+        <v>0.9742897178729163</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B17">
-        <v>17939</v>
+        <v>26466</v>
       </c>
       <c r="C17">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D17">
-        <v>96.73484845631828</v>
+        <v>95.93493740407753</v>
       </c>
       <c r="E17">
-        <v>0.1308979643151661</v>
+        <v>0.9675374918130697</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B18">
-        <v>22203</v>
+        <v>5147</v>
       </c>
       <c r="C18">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D18">
-        <v>96.65951437425936</v>
+        <v>96.32464961255481</v>
       </c>
       <c r="E18">
-        <v>0.2096910634249906</v>
+        <v>0.5599313747988631</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B19">
-        <v>26466</v>
+        <v>9411</v>
       </c>
       <c r="C19">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D19">
-        <v>95.80697390603349</v>
+        <v>96.35253559389359</v>
       </c>
       <c r="E19">
-        <v>1.101376523341193</v>
+        <v>0.530764989129175</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B20">
-        <v>5147</v>
+        <v>13675</v>
       </c>
       <c r="C20">
         <v>95</v>
       </c>
       <c r="D20">
-        <v>95.8966790792869</v>
+        <v>96.38247844608965</v>
       </c>
       <c r="E20">
-        <v>1.007552474336466</v>
+        <v>0.4994472899386575</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B21">
-        <v>9411</v>
+        <v>17939</v>
       </c>
       <c r="C21">
         <v>95</v>
       </c>
       <c r="D21">
-        <v>95.90568450751066</v>
+        <v>96.38551062268573</v>
       </c>
       <c r="E21">
-        <v>0.9981335555792762</v>
+        <v>0.496275888834092</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B22">
-        <v>13675</v>
+        <v>5147</v>
       </c>
       <c r="C22">
         <v>95</v>
       </c>
       <c r="D22">
-        <v>95.91581714251014</v>
+        <v>94.38244608998632</v>
       </c>
       <c r="E22">
-        <v>0.9875356735591134</v>
+        <v>2.59131253008439</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B23">
-        <v>17939</v>
+        <v>9411</v>
       </c>
       <c r="C23">
         <v>95</v>
       </c>
       <c r="D23">
-        <v>95.92117144678738</v>
+        <v>94.374125400975</v>
       </c>
       <c r="E23">
-        <v>0.9819355226572629</v>
+        <v>2.600015269349429</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B24">
-        <v>22203</v>
+        <v>13675</v>
       </c>
       <c r="C24">
         <v>95</v>
       </c>
       <c r="D24">
-        <v>95.9284816007417</v>
+        <v>94.35045094903241</v>
       </c>
       <c r="E24">
-        <v>0.9742897178729163</v>
+        <v>2.624776750306022</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B25">
-        <v>26466</v>
+        <v>17939</v>
       </c>
       <c r="C25">
         <v>95</v>
       </c>
       <c r="D25">
-        <v>95.93493740407753</v>
+        <v>94.35501957496396</v>
       </c>
       <c r="E25">
-        <v>0.9675374918130697</v>
+        <v>2.619998352720463</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B26">
-        <v>5147</v>
+        <v>22203</v>
       </c>
       <c r="C26">
         <v>95</v>
       </c>
       <c r="D26">
-        <v>96.32464961255481</v>
+        <v>94.33667503541776</v>
       </c>
       <c r="E26">
-        <v>0.5599313747988631</v>
+        <v>2.639185194626335</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B27">
-        <v>9411</v>
+        <v>26466</v>
       </c>
       <c r="C27">
         <v>95</v>
       </c>
       <c r="D27">
-        <v>96.35253559389359</v>
+        <v>94.31889937678973</v>
       </c>
       <c r="E27">
-        <v>0.530764989129175</v>
+        <v>2.657777035048911</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B28">
-        <v>13675</v>
+        <v>5147</v>
       </c>
       <c r="C28">
         <v>95</v>
       </c>
       <c r="D28">
-        <v>96.38247844608965</v>
+        <v>96.02705893721442</v>
       </c>
       <c r="E28">
-        <v>0.4994472899386575</v>
+        <v>0.8711861340713126</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B29">
-        <v>17939</v>
+        <v>9411</v>
       </c>
       <c r="C29">
         <v>95</v>
       </c>
       <c r="D29">
-        <v>96.38551062268573</v>
+        <v>96.03311040157466</v>
       </c>
       <c r="E29">
-        <v>0.496275888834092</v>
+        <v>0.8648568124938131</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B30">
-        <v>22203</v>
+        <v>13675</v>
       </c>
       <c r="C30">
         <v>95</v>
       </c>
       <c r="D30">
-        <v>96.34877602775762</v>
+        <v>96.07142216561304</v>
       </c>
       <c r="E30">
-        <v>0.5346971783729421</v>
+        <v>0.8247859370222301</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B31">
-        <v>26466</v>
+        <v>17939</v>
       </c>
       <c r="C31">
         <v>95</v>
       </c>
       <c r="D31">
-        <v>96.36738400263904</v>
+        <v>96.0633668297465</v>
       </c>
       <c r="E31">
-        <v>0.5152348053142592</v>
+        <v>0.8332111392673331</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B32">
-        <v>5147</v>
+        <v>22203</v>
       </c>
       <c r="C32">
         <v>95</v>
       </c>
       <c r="D32">
-        <v>94.38244608998632</v>
+        <v>96.07329493788905</v>
       </c>
       <c r="E32">
-        <v>2.59131253008439</v>
+        <v>0.8228271750977419</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B33">
-        <v>9411</v>
+        <v>26466</v>
       </c>
       <c r="C33">
         <v>95</v>
       </c>
       <c r="D33">
-        <v>94.374125400975</v>
+        <v>96.08678786101692</v>
       </c>
       <c r="E33">
-        <v>2.600015269349429</v>
+        <v>0.8087147149702842</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B34">
-        <v>13675</v>
+        <v>7145</v>
       </c>
       <c r="C34">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D34">
-        <v>94.35045094903241</v>
+        <v>95.96316594272373</v>
       </c>
       <c r="E34">
-        <v>2.624776750306022</v>
+        <v>0.9380128200776731</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B35">
-        <v>17939</v>
+        <v>11409</v>
       </c>
       <c r="C35">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D35">
-        <v>94.35501957496396</v>
+        <v>95.95863835917375</v>
       </c>
       <c r="E35">
-        <v>2.619998352720463</v>
+        <v>0.9427482907920259</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B36">
-        <v>22203</v>
+        <v>15673</v>
       </c>
       <c r="C36">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D36">
-        <v>94.33667503541776</v>
+        <v>95.96858636083584</v>
       </c>
       <c r="E36">
-        <v>2.639185194626335</v>
+        <v>0.9323435196780169</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B37">
-        <v>26466</v>
+        <v>19937</v>
       </c>
       <c r="C37">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D37">
-        <v>94.31889937678973</v>
+        <v>95.97388295008071</v>
       </c>
       <c r="E37">
-        <v>2.657777035048911</v>
+        <v>0.9268037338346269</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B38">
         <v>5147</v>
       </c>
       <c r="C38">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D38">
-        <v>96.02705893721442</v>
+        <v>95.86489972834923</v>
       </c>
       <c r="E38">
-        <v>0.8711861340713126</v>
+        <v>1.040790996392397</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B39">
         <v>9411</v>
       </c>
       <c r="C39">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D39">
-        <v>96.03311040157466</v>
+        <v>95.87643604266033</v>
       </c>
       <c r="E39">
-        <v>0.8648568124938131</v>
+        <v>1.028724984143573</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B40">
         <v>13675</v>
       </c>
       <c r="C40">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D40">
-        <v>96.07142216561304</v>
+        <v>95.88830640324716</v>
       </c>
       <c r="E40">
-        <v>0.8247859370222301</v>
+        <v>1.016309587650702</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B41">
         <v>17939</v>
       </c>
       <c r="C41">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D41">
-        <v>96.0633668297465</v>
+        <v>95.89945413098182</v>
       </c>
       <c r="E41">
-        <v>0.8332111392673331</v>
+        <v>1.004650004202676</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B42">
         <v>22203</v>
       </c>
       <c r="C42">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D42">
-        <v>96.07329493788905</v>
+        <v>95.91007876487561</v>
       </c>
       <c r="E42">
-        <v>0.8228271750977419</v>
+        <v>0.9935375328149757</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B43">
         <v>26466</v>
       </c>
       <c r="C43">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D43">
-        <v>96.08678786101692</v>
+        <v>95.91994819279108</v>
       </c>
       <c r="E43">
-        <v>0.8087147149702842</v>
+        <v>0.983214943216107</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B44">
-        <v>5147</v>
+        <v>7145</v>
       </c>
       <c r="C44">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D44">
-        <v>95.96313148930003</v>
+        <v>95.80624761725565</v>
       </c>
       <c r="E44">
-        <v>0.9380488554544183</v>
+        <v>1.102136160176083</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B45">
-        <v>9411</v>
+        <v>11409</v>
       </c>
       <c r="C45">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D45">
-        <v>95.95997206783568</v>
+        <v>95.80545476259681</v>
       </c>
       <c r="E45">
-        <v>0.9413533439643524</v>
+        <v>1.102965419310942</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B46">
-        <v>13675</v>
+        <v>15673</v>
       </c>
       <c r="C46">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D46">
-        <v>95.96216105821802</v>
+        <v>95.81248396541855</v>
       </c>
       <c r="E46">
-        <v>0.9390638445580901</v>
+        <v>1.095613465726856</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B47">
-        <v>17939</v>
+        <v>19937</v>
       </c>
       <c r="C47">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D47">
-        <v>95.9726784134793</v>
+        <v>95.82011573698951</v>
       </c>
       <c r="E47">
-        <v>0.9280635775763044</v>
+        <v>1.087631276028133</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B48">
-        <v>22203</v>
+        <v>24201</v>
       </c>
       <c r="C48">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D48">
-        <v>95.97743238505245</v>
+        <v>95.82980801346801</v>
       </c>
       <c r="E48">
-        <v>0.9230913240744096</v>
+        <v>1.077493971898324</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B49">
-        <v>26466</v>
+        <v>14141</v>
       </c>
       <c r="C49">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D49">
-        <v>95.98567110073064</v>
+        <v>96.79811330638066</v>
       </c>
       <c r="E49">
-        <v>0.9144743220053884</v>
+        <v>0.06472826442771858</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B50">
-        <v>5147</v>
+        <v>18405</v>
       </c>
       <c r="C50">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D50">
-        <v>95.86489972834923</v>
+        <v>96.78949613184231</v>
       </c>
       <c r="E50">
-        <v>1.040790996392397</v>
+        <v>0.07374110256006855</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B51">
-        <v>9411</v>
+        <v>22669</v>
       </c>
       <c r="C51">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D51">
-        <v>95.87643604266033</v>
+        <v>96.79253183077637</v>
       </c>
       <c r="E51">
-        <v>1.028724984143573</v>
+        <v>0.07056601738691828</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B52">
-        <v>13675</v>
+        <v>26933</v>
       </c>
       <c r="C52">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D52">
-        <v>95.88830640324716</v>
+        <v>96.79778146492313</v>
       </c>
       <c r="E52">
-        <v>1.016309587650702</v>
+        <v>0.06507534261779431</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B53">
-        <v>17939</v>
+        <v>7145</v>
       </c>
       <c r="C53">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D53">
-        <v>95.89945413098182</v>
+        <v>96.47379291631951</v>
       </c>
       <c r="E53">
-        <v>1.004650004202676</v>
+        <v>0.4039400519616092</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B54">
-        <v>22203</v>
+        <v>11409</v>
       </c>
       <c r="C54">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D54">
-        <v>95.91007876487561</v>
+        <v>96.50935870208255</v>
       </c>
       <c r="E54">
-        <v>0.9935375328149757</v>
+        <v>0.3667412382778446</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B55">
-        <v>26466</v>
+        <v>15673</v>
       </c>
       <c r="C55">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D55">
-        <v>95.91994819279108</v>
+        <v>96.53648099073008</v>
       </c>
       <c r="E55">
-        <v>0.983214943216107</v>
+        <v>0.3383736107833045</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B56">
-        <v>5147</v>
+        <v>19937</v>
       </c>
       <c r="C56">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D56">
-        <v>96.62541465520346</v>
+        <v>96.5265843810968</v>
       </c>
       <c r="E56">
-        <v>0.2453564949236949</v>
+        <v>0.3487246301675597</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B57">
-        <v>9411</v>
+        <v>24201</v>
       </c>
       <c r="C57">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D57">
-        <v>96.61768531136876</v>
+        <v>96.53792823815408</v>
       </c>
       <c r="E57">
-        <v>0.2534407369848741</v>
+        <v>0.3368599119819308</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B58">
-        <v>13675</v>
+        <v>17139</v>
       </c>
       <c r="C58">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D58">
-        <v>96.62791536361415</v>
+        <v>96.7443532990423</v>
       </c>
       <c r="E58">
-        <v>0.2427409647378332</v>
+        <v>0.1209567000917293</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B59">
-        <v>17939</v>
+        <v>21403</v>
       </c>
       <c r="C59">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D59">
-        <v>96.6104255177346</v>
+        <v>96.79616615214404</v>
       </c>
       <c r="E59">
-        <v>0.2610338691197645</v>
+        <v>0.06676482361255433</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B60">
-        <v>22203</v>
+        <v>25667</v>
       </c>
       <c r="C60">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D60">
-        <v>96.64084929945784</v>
+        <v>96.78586598219715</v>
       </c>
       <c r="E60">
-        <v>0.2292131581865496</v>
+        <v>0.0775379330643672</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B61">
-        <v>26466</v>
+        <v>5147</v>
       </c>
       <c r="C61">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D61">
-        <v>96.64644763580561</v>
+        <v>96.21650186977092</v>
       </c>
       <c r="E61">
-        <v>0.2233577703110386</v>
+        <v>0.6730447968089845</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B62">
-        <v>5147</v>
+        <v>9411</v>
       </c>
       <c r="C62">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D62">
-        <v>95.8082229430734</v>
+        <v>96.22291099812425</v>
       </c>
       <c r="E62">
-        <v>1.100070135892265</v>
+        <v>0.6663413888460984</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B63">
-        <v>9411</v>
+        <v>13675</v>
       </c>
       <c r="C63">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D63">
-        <v>95.80544406072519</v>
+        <v>96.23013564900805</v>
       </c>
       <c r="E63">
-        <v>1.102976612566476</v>
+        <v>0.6587850130655299</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B64">
-        <v>13675</v>
+        <v>17939</v>
       </c>
       <c r="C64">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D64">
-        <v>95.80825905932554</v>
+        <v>96.23808050908997</v>
       </c>
       <c r="E64">
-        <v>1.100032361337165</v>
+        <v>0.6504753591779396</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B65">
-        <v>17939</v>
+        <v>22203</v>
       </c>
       <c r="C65">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D65">
-        <v>95.81646933167808</v>
+        <v>96.24703453079884</v>
       </c>
       <c r="E65">
-        <v>1.091445108588983</v>
+        <v>0.6411102073017007</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B66">
-        <v>22203</v>
+        <v>26466</v>
       </c>
       <c r="C66">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D66">
-        <v>95.8250367923721</v>
+        <v>96.2559024446147</v>
       </c>
       <c r="E66">
-        <v>1.082484266946859</v>
+        <v>0.6318351170225931</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B67">
-        <v>26466</v>
+        <v>5147</v>
       </c>
       <c r="C67">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D67">
-        <v>95.83485275756571</v>
+        <v>96.34587238823562</v>
       </c>
       <c r="E67">
-        <v>1.072217594848117</v>
+        <v>0.5377341405338069</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B68">
-        <v>7579</v>
+        <v>9411</v>
       </c>
       <c r="C68">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D68">
-        <v>96.79007199358139</v>
+        <v>96.34607278936215</v>
       </c>
       <c r="E68">
-        <v>0.07313879972660807</v>
+        <v>0.5375245378494301</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B69">
-        <v>11843</v>
+        <v>13675</v>
       </c>
       <c r="C69">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D69">
-        <v>96.76785884265448</v>
+        <v>96.34650621611431</v>
       </c>
       <c r="E69">
-        <v>0.09637188300963945</v>
+        <v>0.5370712100049009</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B70">
-        <v>16107</v>
+        <v>17939</v>
       </c>
       <c r="C70">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D70">
-        <v>96.79350281781329</v>
+        <v>96.34791845701795</v>
       </c>
       <c r="E70">
-        <v>0.06955044680128054</v>
+        <v>0.5355941250727335</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B71">
-        <v>20370</v>
+        <v>22203</v>
       </c>
       <c r="C71">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D71">
-        <v>96.7901166545974</v>
+        <v>96.34779699342164</v>
       </c>
       <c r="E71">
-        <v>0.07309208806882042</v>
+        <v>0.5357211657550001</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B72">
-        <v>24634</v>
+        <v>26466</v>
       </c>
       <c r="C72">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D72">
-        <v>96.79519233004679</v>
+        <v>96.34837478541881</v>
       </c>
       <c r="E72">
-        <v>0.06778335943228841</v>
+        <v>0.535116844034297</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B73">
-        <v>5147</v>
+        <v>10143</v>
       </c>
       <c r="C73">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D73">
-        <v>96.39103998641355</v>
+        <v>95.56692547817127</v>
       </c>
       <c r="E73">
-        <v>0.4904926405046</v>
+        <v>1.352446942609269</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B74">
-        <v>9411</v>
+        <v>14407</v>
       </c>
       <c r="C74">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D74">
-        <v>96.48294430466989</v>
+        <v>95.50532931740911</v>
       </c>
       <c r="E74">
-        <v>0.3943684712165216</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="A75" t="s">
-        <v>17</v>
-      </c>
-      <c r="B75">
-        <v>13675</v>
-      </c>
-      <c r="C75">
-        <v>98</v>
-      </c>
-      <c r="D75">
-        <v>96.5287635257519</v>
-      </c>
-      <c r="E75">
-        <v>0.3464454285619738</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" t="s">
-        <v>17</v>
-      </c>
-      <c r="B76">
-        <v>17939</v>
-      </c>
-      <c r="C76">
-        <v>98</v>
-      </c>
-      <c r="D76">
-        <v>96.53232907388093</v>
-      </c>
-      <c r="E76">
-        <v>0.3427161657975817</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" t="s">
-        <v>17</v>
-      </c>
-      <c r="B77">
-        <v>22203</v>
-      </c>
-      <c r="C77">
-        <v>98</v>
-      </c>
-      <c r="D77">
-        <v>96.5312478481794</v>
-      </c>
-      <c r="E77">
-        <v>0.3438470367331852</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" t="s">
-        <v>17</v>
-      </c>
-      <c r="B78">
-        <v>26466</v>
-      </c>
-      <c r="C78">
-        <v>98</v>
-      </c>
-      <c r="D78">
-        <v>96.54327610165387</v>
-      </c>
-      <c r="E78">
-        <v>0.3312664975903486</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" t="s">
-        <v>18</v>
-      </c>
-      <c r="B79">
-        <v>5147</v>
-      </c>
-      <c r="C79">
-        <v>98</v>
-      </c>
-      <c r="D79">
-        <v>96.8107181666457</v>
-      </c>
-      <c r="E79">
-        <v>0.05154464319035816</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
-      <c r="A80" t="s">
-        <v>18</v>
-      </c>
-      <c r="B80">
-        <v>9411</v>
-      </c>
-      <c r="C80">
-        <v>98</v>
-      </c>
-      <c r="D80">
-        <v>96.79601910636498</v>
-      </c>
-      <c r="E80">
-        <v>0.06691862110136548</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
-      <c r="A81" t="s">
-        <v>18</v>
-      </c>
-      <c r="B81">
-        <v>13675</v>
-      </c>
-      <c r="C81">
-        <v>98</v>
-      </c>
-      <c r="D81">
-        <v>96.78882348182179</v>
-      </c>
-      <c r="E81">
-        <v>0.07444463777659441</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
-      <c r="A82" t="s">
-        <v>18</v>
-      </c>
-      <c r="B82">
-        <v>17939</v>
-      </c>
-      <c r="C82">
-        <v>98</v>
-      </c>
-      <c r="D82">
-        <v>96.74757077831148</v>
-      </c>
-      <c r="E82">
-        <v>0.1175914880122529</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
-      <c r="A83" t="s">
-        <v>18</v>
-      </c>
-      <c r="B83">
-        <v>22203</v>
-      </c>
-      <c r="C83">
-        <v>98</v>
-      </c>
-      <c r="D83">
-        <v>96.80324304550834</v>
-      </c>
-      <c r="E83">
-        <v>0.05936298974130141</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
-      <c r="A84" t="s">
-        <v>18</v>
-      </c>
-      <c r="B84">
-        <v>26466</v>
-      </c>
-      <c r="C84">
-        <v>98</v>
-      </c>
-      <c r="D84">
-        <v>96.77671351769273</v>
-      </c>
-      <c r="E84">
-        <v>0.08711063937587932</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
-      <c r="A85" t="s">
-        <v>19</v>
-      </c>
-      <c r="B85">
-        <v>5147</v>
-      </c>
-      <c r="C85">
-        <v>98</v>
-      </c>
-      <c r="D85">
-        <v>96.21650186977092</v>
-      </c>
-      <c r="E85">
-        <v>0.6730447968089845</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
-      <c r="A86" t="s">
-        <v>19</v>
-      </c>
-      <c r="B86">
-        <v>9411</v>
-      </c>
-      <c r="C86">
-        <v>98</v>
-      </c>
-      <c r="D86">
-        <v>96.22291099812425</v>
-      </c>
-      <c r="E86">
-        <v>0.6663413888460984</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
-      <c r="A87" t="s">
-        <v>19</v>
-      </c>
-      <c r="B87">
-        <v>13675</v>
-      </c>
-      <c r="C87">
-        <v>98</v>
-      </c>
-      <c r="D87">
-        <v>96.23013564900805</v>
-      </c>
-      <c r="E87">
-        <v>0.6587850130655299</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
-      <c r="A88" t="s">
-        <v>19</v>
-      </c>
-      <c r="B88">
-        <v>17939</v>
-      </c>
-      <c r="C88">
-        <v>98</v>
-      </c>
-      <c r="D88">
-        <v>96.23808050908997</v>
-      </c>
-      <c r="E88">
-        <v>0.6504753591779396</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
-      <c r="A89" t="s">
-        <v>19</v>
-      </c>
-      <c r="B89">
-        <v>22203</v>
-      </c>
-      <c r="C89">
-        <v>98</v>
-      </c>
-      <c r="D89">
-        <v>96.24703453079884</v>
-      </c>
-      <c r="E89">
-        <v>0.6411102073017007</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
-      <c r="A90" t="s">
-        <v>19</v>
-      </c>
-      <c r="B90">
-        <v>26466</v>
-      </c>
-      <c r="C90">
-        <v>98</v>
-      </c>
-      <c r="D90">
-        <v>96.2559024446147</v>
-      </c>
-      <c r="E90">
-        <v>0.6318351170225931</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
-      <c r="A91" t="s">
-        <v>20</v>
-      </c>
-      <c r="B91">
-        <v>5147</v>
-      </c>
-      <c r="C91">
-        <v>99</v>
-      </c>
-      <c r="D91">
-        <v>95.90687086878079</v>
-      </c>
-      <c r="E91">
-        <v>0.996892721701934</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
-      <c r="A92" t="s">
-        <v>20</v>
-      </c>
-      <c r="B92">
-        <v>9411</v>
-      </c>
-      <c r="C92">
-        <v>99</v>
-      </c>
-      <c r="D92">
-        <v>95.90521518656016</v>
-      </c>
-      <c r="E92">
-        <v>0.9986244257293688</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5">
-      <c r="A93" t="s">
-        <v>20</v>
-      </c>
-      <c r="B93">
-        <v>13675</v>
-      </c>
-      <c r="C93">
-        <v>99</v>
-      </c>
-      <c r="D93">
-        <v>95.90539228159302</v>
-      </c>
-      <c r="E93">
-        <v>0.9984391992542375</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
-      <c r="A94" t="s">
-        <v>20</v>
-      </c>
-      <c r="B94">
-        <v>17939</v>
-      </c>
-      <c r="C94">
-        <v>99</v>
-      </c>
-      <c r="D94">
-        <v>95.90755378568839</v>
-      </c>
-      <c r="E94">
-        <v>0.9961784481870133</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
-      <c r="A95" t="s">
-        <v>20</v>
-      </c>
-      <c r="B95">
-        <v>22203</v>
-      </c>
-      <c r="C95">
-        <v>99</v>
-      </c>
-      <c r="D95">
-        <v>95.91153535922233</v>
-      </c>
-      <c r="E95">
-        <v>0.9920140579203744</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5">
-      <c r="A96" t="s">
-        <v>20</v>
-      </c>
-      <c r="B96">
-        <v>26466</v>
-      </c>
-      <c r="C96">
-        <v>99</v>
-      </c>
-      <c r="D96">
-        <v>95.91384308393128</v>
-      </c>
-      <c r="E96">
-        <v>0.9896003724178605</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
-      <c r="A97" t="s">
-        <v>21</v>
-      </c>
-      <c r="B97">
-        <v>5147</v>
-      </c>
-      <c r="C97">
-        <v>99</v>
-      </c>
-      <c r="D97">
-        <v>96.34587238823562</v>
-      </c>
-      <c r="E97">
-        <v>0.5377341405338069</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
-      <c r="A98" t="s">
-        <v>21</v>
-      </c>
-      <c r="B98">
-        <v>9411</v>
-      </c>
-      <c r="C98">
-        <v>99</v>
-      </c>
-      <c r="D98">
-        <v>96.34607278936215</v>
-      </c>
-      <c r="E98">
-        <v>0.5375245378494301</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
-      <c r="A99" t="s">
-        <v>21</v>
-      </c>
-      <c r="B99">
-        <v>13675</v>
-      </c>
-      <c r="C99">
-        <v>99</v>
-      </c>
-      <c r="D99">
-        <v>96.34650621611431</v>
-      </c>
-      <c r="E99">
-        <v>0.5370712100049009</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5">
-      <c r="A100" t="s">
-        <v>21</v>
-      </c>
-      <c r="B100">
-        <v>17939</v>
-      </c>
-      <c r="C100">
-        <v>99</v>
-      </c>
-      <c r="D100">
-        <v>96.34791845701795</v>
-      </c>
-      <c r="E100">
-        <v>0.5355941250727335</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5">
-      <c r="A101" t="s">
-        <v>21</v>
-      </c>
-      <c r="B101">
-        <v>22203</v>
-      </c>
-      <c r="C101">
-        <v>99</v>
-      </c>
-      <c r="D101">
-        <v>96.34779699342164</v>
-      </c>
-      <c r="E101">
-        <v>0.5357211657550001</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5">
-      <c r="A102" t="s">
-        <v>21</v>
-      </c>
-      <c r="B102">
-        <v>26466</v>
-      </c>
-      <c r="C102">
-        <v>99</v>
-      </c>
-      <c r="D102">
-        <v>96.34837478541881</v>
-      </c>
-      <c r="E102">
-        <v>0.535116844034297</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5">
-      <c r="A103" t="s">
-        <v>22</v>
-      </c>
-      <c r="B103">
-        <v>5147</v>
-      </c>
-      <c r="C103">
-        <v>99</v>
-      </c>
-      <c r="D103">
-        <v>95.71667798435934</v>
-      </c>
-      <c r="E103">
-        <v>1.195818445393431</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5">
-      <c r="A104" t="s">
-        <v>22</v>
-      </c>
-      <c r="B104">
-        <v>9411</v>
-      </c>
-      <c r="C104">
-        <v>99</v>
-      </c>
-      <c r="D104">
-        <v>95.59038956280138</v>
-      </c>
-      <c r="E104">
-        <v>1.327905488127417</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5">
-      <c r="A105" t="s">
-        <v>22</v>
-      </c>
-      <c r="B105">
-        <v>13675</v>
-      </c>
-      <c r="C105">
-        <v>99</v>
-      </c>
-      <c r="D105">
-        <v>95.51035152764447</v>
-      </c>
-      <c r="E105">
-        <v>1.41161852563072</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5">
-      <c r="A106" t="s">
-        <v>22</v>
-      </c>
-      <c r="B106">
-        <v>17939</v>
-      </c>
-      <c r="C106">
-        <v>99</v>
-      </c>
-      <c r="D106">
-        <v>95.67848718354755</v>
-      </c>
-      <c r="E106">
-        <v>1.235762803527306</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5">
-      <c r="A107" t="s">
-        <v>22</v>
-      </c>
-      <c r="B107">
-        <v>22203</v>
-      </c>
-      <c r="C107">
-        <v>99</v>
-      </c>
-      <c r="D107">
-        <v>95.75393973758642</v>
-      </c>
-      <c r="E107">
-        <v>1.156845792713707</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5">
-      <c r="A108" t="s">
-        <v>22</v>
-      </c>
-      <c r="B108">
-        <v>26466</v>
-      </c>
-      <c r="C108">
-        <v>99</v>
-      </c>
-      <c r="D108">
-        <v>95.85655983181788</v>
-      </c>
-      <c r="E108">
-        <v>1.049513825104201</v>
+        <v>1.416871334160542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>